<commit_message>
Update students and teacherts.
</commit_message>
<xml_diff>
--- a/sheet_engine/test_sheets/classes.xlsx
+++ b/sheet_engine/test_sheets/classes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeLab\Projects\curie\sheet_engine\test_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF35246-D05E-409F-A102-1516F4CB9C41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFFB5F4-CA83-47FF-B6BD-550DCBDBDBF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{12C8601B-5275-40A5-A278-1F06C16B1191}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>NAME</t>
   </si>
   <si>
-    <t>1 General Science B</t>
-  </si>
-  <si>
     <t>1 General Arts A</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t>GA11</t>
   </si>
   <si>
-    <t>SC11</t>
-  </si>
-  <si>
     <t>GA</t>
   </si>
   <si>
@@ -84,6 +78,27 @@
   </si>
   <si>
     <t>FORM</t>
+  </si>
+  <si>
+    <t>GA12</t>
+  </si>
+  <si>
+    <t>1 General Arts B</t>
+  </si>
+  <si>
+    <t>1 General Science A</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>1 Business A</t>
+  </si>
+  <si>
+    <t>BUS</t>
+  </si>
+  <si>
+    <t>SCI11</t>
   </si>
 </sst>
 </file>
@@ -146,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -162,6 +177,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -535,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C80F8C-4D44-41FF-97B8-8FD7C8D05CB7}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,200 +567,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="A9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
     </row>
     <row r="10" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
+      <c r="A10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="H11" s="2"/>
     </row>
@@ -753,49 +769,92 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12">
-        <v>1120</v>
+      <c r="E12" s="7">
+        <v>110</v>
       </c>
       <c r="F12" s="3">
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
         <v>2</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>110</v>
+      <c r="B13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="7">
+        <v>111</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" t="s">
-        <v>8</v>
+      <c r="G13" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F14" s="3"/>
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="7">
+        <v>112</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="7">
+        <v>113</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>